<commit_message>
adjust dirs name and merge them
</commit_message>
<xml_diff>
--- a/data/books/index.xlsx
+++ b/data/books/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pycharmProjects\LLMs-JUDGE\data\books\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB21ACC-331E-4419-920A-50D0496FAEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F608AEDC-DD6B-429D-91FC-D7299071222E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="278">
-  <si>
-    <t>书名</t>
-  </si>
-  <si>
-    <t>作者</t>
-  </si>
-  <si>
-    <t>Goodreads 评分</t>
-  </si>
-  <si>
-    <t>Ratings 数</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="279">
   <si>
     <t>Fourth Wing (The Empyrean, #1)</t>
   </si>
@@ -150,9 +138,6 @@
     <t>Abraham Verghese</t>
   </si>
   <si>
-    <t>The Women</t>
-  </si>
-  <si>
     <t>Kristin Hannah</t>
   </si>
   <si>
@@ -333,9 +318,6 @@
     <t>The Tenant</t>
   </si>
   <si>
-    <t>Say You'll Remember Me (Say You'll Remember Me, #1)</t>
-  </si>
-  <si>
     <t>Broken Country</t>
   </si>
   <si>
@@ -385,9 +367,6 @@
   </si>
   <si>
     <t>Reckless (Chestnut Springs, #4)</t>
-  </si>
-  <si>
-    <t>King of Pride (Kings of Sin, #2)</t>
   </si>
   <si>
     <t>Ana Huang</t>
@@ -928,6 +907,37 @@
   </si>
   <si>
     <t>Wild child Wren agrees to a marriage of convenience with her stoic best friend in a move that’s supposed to be practical and temporary. Life on the Rose Hill ranch, shared chores and simmering attraction quickly complicate things, turning a sensible arrangement into a messy, heartfelt love story about choosing your person again and again.</t>
+  </si>
+  <si>
+    <t>The Women</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Say You'll Remember Me</t>
+  </si>
+  <si>
+    <t>King of Pride (Kings of Sin, #2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Freida McFadden</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Author</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoodreadsRatings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RatingsCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1071,7 +1081,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Goodreads 评分</c:v>
+                  <c:v>GoodreadsRatings</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1659,7 +1669,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ratings 数</c:v>
+                  <c:v>RatingsCount</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3643,40 +3653,41 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.75" customWidth="1"/>
+    <col min="1" max="1" width="48.375" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>276</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>277</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>177</v>
+        <v>278</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>4.57</v>
@@ -3684,17 +3695,17 @@
       <c r="D2" s="1">
         <v>3392074</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>178</v>
+      <c r="E2" s="3" t="s">
+        <v>171</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>4.3600000000000003</v>
@@ -3702,17 +3713,17 @@
       <c r="D3" s="1">
         <v>2491239</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>179</v>
+      <c r="E3" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>3.94</v>
@@ -3720,17 +3731,17 @@
       <c r="D4" s="1">
         <v>1390059</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>180</v>
+      <c r="E4" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>4.18</v>
@@ -3738,17 +3749,17 @@
       <c r="D5" s="1">
         <v>1500376</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>181</v>
+      <c r="E5" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>4.16</v>
@@ -3756,17 +3767,17 @@
       <c r="D6" s="1">
         <v>883117</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>182</v>
+      <c r="E6" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>3.73</v>
@@ -3774,17 +3785,17 @@
       <c r="D7" s="1">
         <v>993005</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>183</v>
+      <c r="E7" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>4.08</v>
@@ -3792,17 +3803,17 @@
       <c r="D8" s="1">
         <v>1064333</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>184</v>
+      <c r="E8" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>4.1500000000000004</v>
@@ -3810,17 +3821,17 @@
       <c r="D9" s="1">
         <v>717525</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>185</v>
+      <c r="E9" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>4.3</v>
@@ -3828,17 +3839,17 @@
       <c r="D10" s="1">
         <v>798995</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>186</v>
+      <c r="E10" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>4.17</v>
@@ -3846,17 +3857,17 @@
       <c r="D11" s="1">
         <v>562637</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>187</v>
+      <c r="E11" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>4.08</v>
@@ -3864,17 +3875,17 @@
       <c r="D12" s="1">
         <v>644608</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>188</v>
+      <c r="E12" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>4.01</v>
@@ -3882,17 +3893,17 @@
       <c r="D13" s="1">
         <v>592813</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>189</v>
+      <c r="E13" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C14">
         <v>4.13</v>
@@ -3900,17 +3911,17 @@
       <c r="D14" s="1">
         <v>527854</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>190</v>
+      <c r="E14" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>4.03</v>
@@ -3918,17 +3929,17 @@
       <c r="D15" s="1">
         <v>514439</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>191</v>
+      <c r="E15" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C16">
         <v>4.13</v>
@@ -3936,17 +3947,17 @@
       <c r="D16" s="1">
         <v>582971</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>192</v>
+      <c r="E16" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>4.38</v>
@@ -3954,17 +3965,17 @@
       <c r="D17" s="1">
         <v>495558</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>193</v>
+      <c r="E17" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>3.93</v>
@@ -3972,17 +3983,17 @@
       <c r="D18" s="1">
         <v>484285</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>194</v>
+      <c r="E18" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19">
         <v>4.0599999999999996</v>
@@ -3990,17 +4001,17 @@
       <c r="D19" s="1">
         <v>384432</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>195</v>
+      <c r="E19" s="3" t="s">
+        <v>188</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>4.41</v>
@@ -4008,17 +4019,17 @@
       <c r="D20" s="1">
         <v>302745</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>196</v>
+      <c r="E20" s="3" t="s">
+        <v>189</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>271</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>4.59</v>
@@ -4026,17 +4037,17 @@
       <c r="D21" s="1">
         <v>1488645</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>197</v>
+      <c r="E21" s="3" t="s">
+        <v>190</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>4.1900000000000004</v>
@@ -4044,17 +4055,17 @@
       <c r="D22" s="1">
         <v>1230155</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>198</v>
+      <c r="E22" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>4.08</v>
@@ -4062,17 +4073,17 @@
       <c r="D23" s="1">
         <v>935991</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>199</v>
+      <c r="E23" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C24">
         <v>4.3499999999999996</v>
@@ -4080,17 +4091,17 @@
       <c r="D24" s="1">
         <v>1036492</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>200</v>
+      <c r="E24" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>4.1100000000000003</v>
@@ -4098,17 +4109,17 @@
       <c r="D25" s="1">
         <v>725057</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>201</v>
+      <c r="E25" s="3" t="s">
+        <v>194</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C26">
         <v>3.86</v>
@@ -4116,17 +4127,17 @@
       <c r="D26" s="1">
         <v>875229</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>202</v>
+      <c r="E26" s="3" t="s">
+        <v>195</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>274</v>
       </c>
       <c r="C27">
         <v>3.89</v>
@@ -4134,17 +4145,17 @@
       <c r="D27" s="1">
         <v>924104</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>203</v>
+      <c r="E27" s="3" t="s">
+        <v>196</v>
       </c>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>4.2300000000000004</v>
@@ -4152,17 +4163,17 @@
       <c r="D28" s="1">
         <v>656419</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>204</v>
+      <c r="E28" s="3" t="s">
+        <v>197</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -4170,17 +4181,17 @@
       <c r="D29" s="1">
         <v>661300</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>205</v>
+      <c r="E29" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>3.82</v>
@@ -4188,17 +4199,17 @@
       <c r="D30" s="1">
         <v>319424</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>206</v>
+      <c r="E30" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>4.21</v>
@@ -4206,17 +4217,17 @@
       <c r="D31" s="1">
         <v>1553466</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>207</v>
+      <c r="E31" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C32">
         <v>4.07</v>
@@ -4224,17 +4235,17 @@
       <c r="D32" s="1">
         <v>459730</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>208</v>
+      <c r="E32" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>3.81</v>
@@ -4242,17 +4253,17 @@
       <c r="D33" s="1">
         <v>459007</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>209</v>
+      <c r="E33" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C34">
         <v>3.92</v>
@@ -4260,17 +4271,17 @@
       <c r="D34" s="1">
         <v>313196</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>210</v>
+      <c r="E34" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <v>4.3899999999999997</v>
@@ -4278,17 +4289,17 @@
       <c r="D35" s="1">
         <v>467158</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>211</v>
+      <c r="E35" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C36">
         <v>4.3899999999999997</v>
@@ -4296,17 +4307,17 @@
       <c r="D36" s="1">
         <v>434199</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>212</v>
+      <c r="E36" s="3" t="s">
+        <v>205</v>
       </c>
       <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C37">
         <v>3.93</v>
@@ -4314,17 +4325,17 @@
       <c r="D37" s="1">
         <v>321374</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>213</v>
+      <c r="E37" s="3" t="s">
+        <v>206</v>
       </c>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>4.5999999999999996</v>
@@ -4332,17 +4343,17 @@
       <c r="D38" s="1">
         <v>174566</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>214</v>
+      <c r="E38" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C39">
         <v>4.16</v>
@@ -4350,17 +4361,17 @@
       <c r="D39" s="1">
         <v>395153</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>215</v>
+      <c r="E39" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C40">
         <v>3.94</v>
@@ -4368,17 +4379,17 @@
       <c r="D40" s="1">
         <v>348866</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>216</v>
+      <c r="E40" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -4386,17 +4397,17 @@
       <c r="D41" s="1">
         <v>331158</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>217</v>
+      <c r="E41" s="3" t="s">
+        <v>210</v>
       </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C42">
         <v>4.1100000000000003</v>
@@ -4404,17 +4415,17 @@
       <c r="D42" s="1">
         <v>541256</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>218</v>
+      <c r="E42" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C43">
         <v>4.4400000000000004</v>
@@ -4422,17 +4433,17 @@
       <c r="D43" s="1">
         <v>463564</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>219</v>
+      <c r="E43" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>4.07</v>
@@ -4440,17 +4451,17 @@
       <c r="D44" s="1">
         <v>556473</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>220</v>
+      <c r="E44" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C45">
         <v>4.25</v>
@@ -4458,17 +4469,17 @@
       <c r="D45" s="1">
         <v>423860</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>221</v>
+      <c r="E45" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C46">
         <v>3.99</v>
@@ -4476,17 +4487,17 @@
       <c r="D46" s="1">
         <v>275014</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>222</v>
+      <c r="E46" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C47">
         <v>4.17</v>
@@ -4494,17 +4505,17 @@
       <c r="D47" s="1">
         <v>364435</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>223</v>
+      <c r="E47" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="G47" s="3"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B48" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C48">
         <v>4</v>
@@ -4512,17 +4523,17 @@
       <c r="D48" s="1">
         <v>409065</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>224</v>
+      <c r="E48" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C49">
         <v>4.07</v>
@@ -4530,17 +4541,17 @@
       <c r="D49" s="1">
         <v>494198</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>225</v>
+      <c r="E49" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C50">
         <v>4.07</v>
@@ -4548,17 +4559,17 @@
       <c r="D50" s="1">
         <v>428231</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>226</v>
+      <c r="E50" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C51">
         <v>3.92</v>
@@ -4566,17 +4577,17 @@
       <c r="D51" s="1">
         <v>277372</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>227</v>
+      <c r="E51" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C52">
         <v>4.51</v>
@@ -4584,17 +4595,17 @@
       <c r="D52" s="1">
         <v>951131</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>228</v>
+      <c r="E52" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C53">
         <v>3.97</v>
@@ -4602,17 +4613,17 @@
       <c r="D53" s="1">
         <v>602120</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>229</v>
+      <c r="E53" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C54">
         <v>4.34</v>
@@ -4620,17 +4631,17 @@
       <c r="D54" s="1">
         <v>512807</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>230</v>
+      <c r="E54" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>3.69</v>
@@ -4638,17 +4649,17 @@
       <c r="D55" s="1">
         <v>510317</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>231</v>
+      <c r="E55" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="G55" s="3"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C56">
         <v>3.83</v>
@@ -4656,17 +4667,17 @@
       <c r="D56" s="1">
         <v>485774</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>232</v>
+      <c r="E56" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>272</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C57">
         <v>4.0199999999999996</v>
@@ -4674,17 +4685,17 @@
       <c r="D57" s="1">
         <v>435572</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>233</v>
+      <c r="E57" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="G57" s="3"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C58">
         <v>4.3099999999999996</v>
@@ -4692,17 +4703,17 @@
       <c r="D58" s="1">
         <v>370923</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>234</v>
+      <c r="E58" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C59">
         <v>3.87</v>
@@ -4710,17 +4721,17 @@
       <c r="D59" s="1">
         <v>408825</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>235</v>
+      <c r="E59" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C60">
         <v>4.3</v>
@@ -4728,17 +4739,17 @@
       <c r="D60" s="1">
         <v>372839</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>236</v>
+      <c r="E60" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="G60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C61">
         <v>4.41</v>
@@ -4746,17 +4757,17 @@
       <c r="D61" s="1">
         <v>258366</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>237</v>
+      <c r="E61" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B62" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C62">
         <v>3.74</v>
@@ -4764,17 +4775,17 @@
       <c r="D62" s="1">
         <v>544980</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>238</v>
+      <c r="E62" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C63">
         <v>3.36</v>
@@ -4782,17 +4793,17 @@
       <c r="D63" s="1">
         <v>516287</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>239</v>
+      <c r="E63" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C64">
         <v>4.3899999999999997</v>
@@ -4800,17 +4811,17 @@
       <c r="D64" s="1">
         <v>408579</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>240</v>
+      <c r="E64" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C65">
         <v>4.17</v>
@@ -4818,17 +4829,17 @@
       <c r="D65" s="1">
         <v>252113</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>241</v>
+      <c r="E65" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C66">
         <v>3.68</v>
@@ -4836,17 +4847,17 @@
       <c r="D66" s="1">
         <v>355469</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>242</v>
+      <c r="E66" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="G66" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C67">
         <v>3.96</v>
@@ -4854,17 +4865,17 @@
       <c r="D67" s="1">
         <v>203157</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>243</v>
+      <c r="E67" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C68">
         <v>4.3600000000000003</v>
@@ -4872,17 +4883,17 @@
       <c r="D68" s="1">
         <v>399180</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>244</v>
+      <c r="E68" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>120</v>
+        <v>273</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C69">
         <v>3.91</v>
@@ -4890,17 +4901,17 @@
       <c r="D69" s="1">
         <v>348096</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>245</v>
+      <c r="E69" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C70">
         <v>4.18</v>
@@ -4908,17 +4919,17 @@
       <c r="D70" s="1">
         <v>304991</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>246</v>
+      <c r="E70" s="3" t="s">
+        <v>239</v>
       </c>
       <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C71">
         <v>4.32</v>
@@ -4926,17 +4937,17 @@
       <c r="D71" s="1">
         <v>272820</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>247</v>
+      <c r="E71" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C72">
         <v>4.05</v>
@@ -4944,17 +4955,17 @@
       <c r="D72" s="1">
         <v>271438</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>248</v>
+      <c r="E72" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C73">
         <v>4.08</v>
@@ -4962,17 +4973,17 @@
       <c r="D73" s="1">
         <v>290145</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>249</v>
+      <c r="E73" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B74" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C74">
         <v>4.01</v>
@@ -4980,17 +4991,17 @@
       <c r="D74" s="1">
         <v>323019</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>250</v>
+      <c r="E74" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="G74" s="3"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C75">
         <v>3.99</v>
@@ -4998,17 +5009,17 @@
       <c r="D75" s="1">
         <v>221983</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>251</v>
+      <c r="E75" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B76" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C76">
         <v>4.34</v>
@@ -5016,17 +5027,17 @@
       <c r="D76" s="1">
         <v>730263</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>252</v>
+      <c r="E76" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="G76" s="3"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B77" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C77">
         <v>4</v>
@@ -5034,17 +5045,17 @@
       <c r="D77" s="1">
         <v>766752</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>253</v>
+      <c r="E77" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C78">
         <v>4.03</v>
@@ -5052,17 +5063,17 @@
       <c r="D78" s="1">
         <v>873108</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>254</v>
+      <c r="E78" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C79">
         <v>4.05</v>
@@ -5070,17 +5081,17 @@
       <c r="D79" s="1">
         <v>291737</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>255</v>
+      <c r="E79" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="G79" s="3"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C80">
         <v>3.95</v>
@@ -5088,17 +5099,17 @@
       <c r="D80" s="1">
         <v>349587</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>256</v>
+      <c r="E80" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="G80" s="3"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B81" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C81">
         <v>3.91</v>
@@ -5106,17 +5117,17 @@
       <c r="D81" s="1">
         <v>179826</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>257</v>
+      <c r="E81" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C82">
         <v>3.64</v>
@@ -5124,17 +5135,17 @@
       <c r="D82" s="1">
         <v>300748</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>258</v>
+      <c r="E82" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="G82" s="3"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C83">
         <v>3.57</v>
@@ -5142,17 +5153,17 @@
       <c r="D83" s="1">
         <v>206155</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>259</v>
+      <c r="E83" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B84" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C84">
         <v>3.8</v>
@@ -5160,17 +5171,17 @@
       <c r="D84" s="1">
         <v>281679</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>260</v>
+      <c r="E84" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B85" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C85">
         <v>3.99</v>
@@ -5178,17 +5189,17 @@
       <c r="D85" s="1">
         <v>276843</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>261</v>
+      <c r="E85" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B86" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C86">
         <v>4.29</v>
@@ -5196,17 +5207,17 @@
       <c r="D86" s="1">
         <v>233564</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>262</v>
+      <c r="E86" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="G86" s="3"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C87">
         <v>3.58</v>
@@ -5214,17 +5225,17 @@
       <c r="D87" s="1">
         <v>257139</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>263</v>
+      <c r="E87" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="G87" s="3"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C88">
         <v>3.63</v>
@@ -5232,17 +5243,17 @@
       <c r="D88" s="1">
         <v>233674</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>264</v>
+      <c r="E88" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B89" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -5250,17 +5261,17 @@
       <c r="D89" s="1">
         <v>286871</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>265</v>
+      <c r="E89" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="G89" s="3"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B90" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C90">
         <v>4.13</v>
@@ -5268,17 +5279,17 @@
       <c r="D90" s="1">
         <v>229757</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>266</v>
+      <c r="E90" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="G90" s="3"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C91">
         <v>4.07</v>
@@ -5286,17 +5297,17 @@
       <c r="D91" s="1">
         <v>330308</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>267</v>
+      <c r="E91" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="G91" s="3"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C92">
         <v>3.6</v>
@@ -5304,17 +5315,17 @@
       <c r="D92" s="1">
         <v>259713</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>268</v>
+      <c r="E92" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="G92" s="3"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B93" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C93">
         <v>4.47</v>
@@ -5322,17 +5333,17 @@
       <c r="D93" s="1">
         <v>103277</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>269</v>
+      <c r="E93" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B94" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C94">
         <v>4.4000000000000004</v>
@@ -5340,17 +5351,17 @@
       <c r="D94" s="1">
         <v>225128</v>
       </c>
-      <c r="F94" s="3" t="s">
-        <v>270</v>
+      <c r="E94" s="3" t="s">
+        <v>263</v>
       </c>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C95">
         <v>4.28</v>
@@ -5358,17 +5369,17 @@
       <c r="D95" s="1">
         <v>149720</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>271</v>
+      <c r="E95" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C96">
         <v>3.98</v>
@@ -5376,17 +5387,17 @@
       <c r="D96" s="1">
         <v>125972</v>
       </c>
-      <c r="F96" s="3" t="s">
-        <v>272</v>
+      <c r="E96" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C97">
         <v>3.91</v>
@@ -5394,17 +5405,17 @@
       <c r="D97" s="1">
         <v>187468</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>273</v>
+      <c r="E97" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="G97" s="3"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B98" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C98">
         <v>4.0199999999999996</v>
@@ -5412,17 +5423,17 @@
       <c r="D98" s="1">
         <v>211843</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>274</v>
+      <c r="E98" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="G98" s="3"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C99">
         <v>3.82</v>
@@ -5430,17 +5441,17 @@
       <c r="D99" s="1">
         <v>83450</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>275</v>
+      <c r="E99" s="3" t="s">
+        <v>268</v>
       </c>
       <c r="G99" s="3"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B100" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C100">
         <v>3.96</v>
@@ -5448,17 +5459,17 @@
       <c r="D100" s="1">
         <v>202541</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>276</v>
+      <c r="E100" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="G100" s="3"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C101">
         <v>4.18</v>
@@ -5466,8 +5477,8 @@
       <c r="D101" s="1">
         <v>215188</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>277</v>
+      <c r="E101" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="G101" s="3"/>
     </row>

</xml_diff>